<commit_message>
template changes paper file example to run well :^)
</commit_message>
<xml_diff>
--- a/genetic-conference/template.xlsx
+++ b/genetic-conference/template.xlsx
@@ -25,7 +25,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -51,6 +51,19 @@
     <font>
       <sz val="11"/>
       <name val="Roboto Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Roboto Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -116,7 +129,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -129,19 +142,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,7 +254,7 @@
   <dimension ref="A1:BC1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="AS38" activeCellId="0" sqref="AS38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -382,7 +407,7 @@
       <c r="BB4" s="4"/>
       <c r="BC4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
@@ -443,7 +468,7 @@
       <c r="BB5" s="4"/>
       <c r="BC5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
@@ -504,7 +529,7 @@
       <c r="BB6" s="4"/>
       <c r="BC6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
@@ -565,7 +590,7 @@
       <c r="BB7" s="4"/>
       <c r="BC7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
@@ -626,7 +651,7 @@
       <c r="BB8" s="4"/>
       <c r="BC8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>5</v>
       </c>
@@ -687,7 +712,7 @@
       <c r="BB9" s="4"/>
       <c r="BC9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>6</v>
       </c>
@@ -748,7 +773,7 @@
       <c r="BB10" s="4"/>
       <c r="BC10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>7</v>
       </c>
@@ -809,7 +834,7 @@
       <c r="BB11" s="4"/>
       <c r="BC11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>8</v>
       </c>
@@ -870,7 +895,7 @@
       <c r="BB12" s="4"/>
       <c r="BC12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>9</v>
       </c>
@@ -931,7 +956,7 @@
       <c r="BB13" s="4"/>
       <c r="BC13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>10</v>
       </c>
@@ -992,7 +1017,7 @@
       <c r="BB14" s="4"/>
       <c r="BC14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>11</v>
       </c>
@@ -1053,7 +1078,7 @@
       <c r="BB15" s="4"/>
       <c r="BC15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>12</v>
       </c>
@@ -1114,7 +1139,7 @@
       <c r="BB16" s="6"/>
       <c r="BC16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>13</v>
       </c>
@@ -1175,7 +1200,7 @@
       <c r="BB17" s="6"/>
       <c r="BC17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>14</v>
       </c>
@@ -1236,199 +1261,373 @@
       <c r="BB18" s="6"/>
       <c r="BC18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
+      <c r="AI19" s="8"/>
+      <c r="AJ19" s="8"/>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
+      <c r="AM19" s="8"/>
+      <c r="AN19" s="8"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="8"/>
+      <c r="AR19" s="8"/>
+      <c r="AS19" s="8"/>
+      <c r="AT19" s="8"/>
+      <c r="AU19" s="8"/>
+      <c r="AV19" s="8"/>
+      <c r="AW19" s="8"/>
+      <c r="AX19" s="8"/>
+      <c r="AY19" s="8"/>
+      <c r="AZ19" s="8"/>
+      <c r="BA19" s="8"/>
+      <c r="BB19" s="8"/>
+      <c r="BC19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>0.486111111111111</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="8"/>
+      <c r="AT20" s="8"/>
+      <c r="AU20" s="8"/>
+      <c r="AV20" s="8"/>
+      <c r="AW20" s="8"/>
+      <c r="AX20" s="8"/>
+      <c r="AY20" s="8"/>
+      <c r="AZ20" s="8"/>
+      <c r="BA20" s="8"/>
+      <c r="BB20" s="8"/>
+      <c r="BC20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>0.493055555555556</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="8"/>
+      <c r="AS21" s="8"/>
+      <c r="AT21" s="8"/>
+      <c r="AU21" s="8"/>
+      <c r="AV21" s="8"/>
+      <c r="AW21" s="8"/>
+      <c r="AX21" s="8"/>
+      <c r="AY21" s="8"/>
+      <c r="AZ21" s="8"/>
+      <c r="BA21" s="8"/>
+      <c r="BB21" s="8"/>
+      <c r="BC21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="8"/>
+      <c r="AN22" s="8"/>
+      <c r="AO22" s="8"/>
+      <c r="AP22" s="8"/>
+      <c r="AQ22" s="8"/>
+      <c r="AR22" s="8"/>
+      <c r="AS22" s="8"/>
+      <c r="AT22" s="8"/>
+      <c r="AU22" s="8"/>
+      <c r="AV22" s="8"/>
+      <c r="AW22" s="8"/>
+      <c r="AX22" s="8"/>
+      <c r="AY22" s="8"/>
+      <c r="AZ22" s="8"/>
+      <c r="BA22" s="8"/>
+      <c r="BB22" s="8"/>
+      <c r="BC22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>0.506944444444444</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8"/>
+      <c r="AN23" s="8"/>
+      <c r="AO23" s="8"/>
+      <c r="AP23" s="8"/>
+      <c r="AQ23" s="8"/>
+      <c r="AR23" s="8"/>
+      <c r="AS23" s="8"/>
+      <c r="AT23" s="8"/>
+      <c r="AU23" s="8"/>
+      <c r="AV23" s="8"/>
+      <c r="AW23" s="8"/>
+      <c r="AX23" s="8"/>
+      <c r="AY23" s="8"/>
+      <c r="AZ23" s="8"/>
+      <c r="BA23" s="8"/>
+      <c r="BB23" s="8"/>
+      <c r="BC23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0.513888888888889</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
+      <c r="AN24" s="8"/>
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="8"/>
+      <c r="AQ24" s="8"/>
+      <c r="AR24" s="8"/>
+      <c r="AS24" s="8"/>
+      <c r="AT24" s="8"/>
+      <c r="AU24" s="8"/>
+      <c r="AV24" s="8"/>
+      <c r="AW24" s="8"/>
+      <c r="AX24" s="8"/>
+      <c r="AY24" s="8"/>
+      <c r="AZ24" s="8"/>
+      <c r="BA24" s="8"/>
+      <c r="BB24" s="8"/>
+      <c r="BC24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>21</v>
       </c>
@@ -1489,7 +1688,7 @@
       <c r="BB25" s="6"/>
       <c r="BC25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>22</v>
       </c>
@@ -1550,7 +1749,7 @@
       <c r="BB26" s="6"/>
       <c r="BC26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>23</v>
       </c>
@@ -1611,7 +1810,7 @@
       <c r="BB27" s="6"/>
       <c r="BC27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>24</v>
       </c>
@@ -1672,7 +1871,7 @@
       <c r="BB28" s="6"/>
       <c r="BC28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>25</v>
       </c>
@@ -1733,7 +1932,7 @@
       <c r="BB29" s="6"/>
       <c r="BC29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>26</v>
       </c>
@@ -1794,7 +1993,7 @@
       <c r="BB30" s="6"/>
       <c r="BC30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>27</v>
       </c>
@@ -1855,7 +2054,7 @@
       <c r="BB31" s="6"/>
       <c r="BC31" s="6"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>28</v>
       </c>
@@ -1916,7 +2115,7 @@
       <c r="BB32" s="6"/>
       <c r="BC32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>29</v>
       </c>
@@ -1977,7 +2176,7 @@
       <c r="BB33" s="6"/>
       <c r="BC33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>30</v>
       </c>
@@ -2038,7 +2237,7 @@
       <c r="BB34" s="4"/>
       <c r="BC34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>31</v>
       </c>
@@ -2099,7 +2298,7 @@
       <c r="BB35" s="4"/>
       <c r="BC35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>32</v>
       </c>
@@ -2160,7 +2359,7 @@
       <c r="BB36" s="4"/>
       <c r="BC36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>33</v>
       </c>
@@ -2221,7 +2420,7 @@
       <c r="BB37" s="4"/>
       <c r="BC37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>34</v>
       </c>
@@ -2282,7 +2481,7 @@
       <c r="BB38" s="4"/>
       <c r="BC38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>35</v>
       </c>
@@ -2343,7 +2542,7 @@
       <c r="BB39" s="4"/>
       <c r="BC39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>36</v>
       </c>
@@ -2404,7 +2603,7 @@
       <c r="BB40" s="4"/>
       <c r="BC40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>37</v>
       </c>
@@ -2465,7 +2664,7 @@
       <c r="BB41" s="4"/>
       <c r="BC41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>38</v>
       </c>
@@ -2526,7 +2725,7 @@
       <c r="BB42" s="4"/>
       <c r="BC42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>39</v>
       </c>
@@ -2587,7 +2786,7 @@
       <c r="BB43" s="4"/>
       <c r="BC43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>40</v>
       </c>
@@ -2648,7 +2847,7 @@
       <c r="BB44" s="4"/>
       <c r="BC44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>41</v>
       </c>
@@ -2709,203 +2908,377 @@
       <c r="BB45" s="4"/>
       <c r="BC45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
-      <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="8"/>
+      <c r="AB46" s="8"/>
+      <c r="AC46" s="8"/>
+      <c r="AD46" s="8"/>
+      <c r="AE46" s="8"/>
+      <c r="AF46" s="8"/>
+      <c r="AG46" s="8"/>
+      <c r="AH46" s="8"/>
+      <c r="AI46" s="8"/>
+      <c r="AJ46" s="8"/>
+      <c r="AK46" s="8"/>
+      <c r="AL46" s="8"/>
+      <c r="AM46" s="8"/>
+      <c r="AN46" s="8"/>
+      <c r="AO46" s="8"/>
+      <c r="AP46" s="8"/>
+      <c r="AQ46" s="8"/>
+      <c r="AR46" s="8"/>
+      <c r="AS46" s="8"/>
+      <c r="AT46" s="8"/>
+      <c r="AU46" s="8"/>
+      <c r="AV46" s="8"/>
+      <c r="AW46" s="8"/>
+      <c r="AX46" s="8"/>
+      <c r="AY46" s="8"/>
+      <c r="AZ46" s="8"/>
+      <c r="BA46" s="8"/>
+      <c r="BB46" s="8"/>
+      <c r="BC46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>43</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>0.673611111111111</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
-      <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="8"/>
+      <c r="AB47" s="8"/>
+      <c r="AC47" s="8"/>
+      <c r="AD47" s="8"/>
+      <c r="AE47" s="8"/>
+      <c r="AF47" s="8"/>
+      <c r="AG47" s="8"/>
+      <c r="AH47" s="8"/>
+      <c r="AI47" s="8"/>
+      <c r="AJ47" s="8"/>
+      <c r="AK47" s="8"/>
+      <c r="AL47" s="8"/>
+      <c r="AM47" s="8"/>
+      <c r="AN47" s="8"/>
+      <c r="AO47" s="8"/>
+      <c r="AP47" s="8"/>
+      <c r="AQ47" s="8"/>
+      <c r="AR47" s="8"/>
+      <c r="AS47" s="8"/>
+      <c r="AT47" s="8"/>
+      <c r="AU47" s="8"/>
+      <c r="AV47" s="8"/>
+      <c r="AW47" s="8"/>
+      <c r="AX47" s="8"/>
+      <c r="AY47" s="8"/>
+      <c r="AZ47" s="8"/>
+      <c r="BA47" s="8"/>
+      <c r="BB47" s="8"/>
+      <c r="BC47" s="8"/>
+    </row>
+    <row r="48" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>44</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>0.680555555555556</v>
       </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-      <c r="W48" s="1"/>
-      <c r="X48" s="1"/>
-      <c r="Y48" s="1"/>
-      <c r="Z48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="8"/>
+      <c r="AB48" s="8"/>
+      <c r="AC48" s="8"/>
+      <c r="AD48" s="8"/>
+      <c r="AE48" s="8"/>
+      <c r="AF48" s="8"/>
+      <c r="AG48" s="8"/>
+      <c r="AH48" s="8"/>
+      <c r="AI48" s="8"/>
+      <c r="AJ48" s="8"/>
+      <c r="AK48" s="8"/>
+      <c r="AL48" s="8"/>
+      <c r="AM48" s="8"/>
+      <c r="AN48" s="8"/>
+      <c r="AO48" s="8"/>
+      <c r="AP48" s="8"/>
+      <c r="AQ48" s="8"/>
+      <c r="AR48" s="8"/>
+      <c r="AS48" s="8"/>
+      <c r="AT48" s="8"/>
+      <c r="AU48" s="8"/>
+      <c r="AV48" s="8"/>
+      <c r="AW48" s="8"/>
+      <c r="AX48" s="8"/>
+      <c r="AY48" s="8"/>
+      <c r="AZ48" s="8"/>
+      <c r="BA48" s="8"/>
+      <c r="BB48" s="8"/>
+      <c r="BC48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>45</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
+      <c r="V49" s="7"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="7"/>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7"/>
+      <c r="AA49" s="8"/>
+      <c r="AB49" s="8"/>
+      <c r="AC49" s="8"/>
+      <c r="AD49" s="8"/>
+      <c r="AE49" s="8"/>
+      <c r="AF49" s="8"/>
+      <c r="AG49" s="8"/>
+      <c r="AH49" s="8"/>
+      <c r="AI49" s="8"/>
+      <c r="AJ49" s="8"/>
+      <c r="AK49" s="8"/>
+      <c r="AL49" s="8"/>
+      <c r="AM49" s="8"/>
+      <c r="AN49" s="8"/>
+      <c r="AO49" s="8"/>
+      <c r="AP49" s="8"/>
+      <c r="AQ49" s="8"/>
+      <c r="AR49" s="8"/>
+      <c r="AS49" s="8"/>
+      <c r="AT49" s="8"/>
+      <c r="AU49" s="8"/>
+      <c r="AV49" s="8"/>
+      <c r="AW49" s="8"/>
+      <c r="AX49" s="8"/>
+      <c r="AY49" s="8"/>
+      <c r="AZ49" s="8"/>
+      <c r="BA49" s="8"/>
+      <c r="BB49" s="8"/>
+      <c r="BC49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>46</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>0.694444444444444</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-      <c r="X50" s="1"/>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="8"/>
+      <c r="AB50" s="8"/>
+      <c r="AC50" s="8"/>
+      <c r="AD50" s="8"/>
+      <c r="AE50" s="8"/>
+      <c r="AF50" s="8"/>
+      <c r="AG50" s="8"/>
+      <c r="AH50" s="8"/>
+      <c r="AI50" s="8"/>
+      <c r="AJ50" s="8"/>
+      <c r="AK50" s="8"/>
+      <c r="AL50" s="8"/>
+      <c r="AM50" s="8"/>
+      <c r="AN50" s="8"/>
+      <c r="AO50" s="8"/>
+      <c r="AP50" s="8"/>
+      <c r="AQ50" s="8"/>
+      <c r="AR50" s="8"/>
+      <c r="AS50" s="8"/>
+      <c r="AT50" s="8"/>
+      <c r="AU50" s="8"/>
+      <c r="AV50" s="8"/>
+      <c r="AW50" s="8"/>
+      <c r="AX50" s="8"/>
+      <c r="AY50" s="8"/>
+      <c r="AZ50" s="8"/>
+      <c r="BA50" s="8"/>
+      <c r="BB50" s="8"/>
+      <c r="BC50" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>0.701388888888889</v>
       </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
-      <c r="V51" s="1"/>
-      <c r="W51" s="1"/>
-      <c r="X51" s="1"/>
-      <c r="Y51" s="1"/>
-      <c r="Z51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
+      <c r="V51" s="7"/>
+      <c r="W51" s="7"/>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="8"/>
+      <c r="AB51" s="8"/>
+      <c r="AC51" s="8"/>
+      <c r="AD51" s="8"/>
+      <c r="AE51" s="8"/>
+      <c r="AF51" s="8"/>
+      <c r="AG51" s="8"/>
+      <c r="AH51" s="8"/>
+      <c r="AI51" s="8"/>
+      <c r="AJ51" s="8"/>
+      <c r="AK51" s="8"/>
+      <c r="AL51" s="8"/>
+      <c r="AM51" s="8"/>
+      <c r="AN51" s="8"/>
+      <c r="AO51" s="8"/>
+      <c r="AP51" s="8"/>
+      <c r="AQ51" s="8"/>
+      <c r="AR51" s="8"/>
+      <c r="AS51" s="8"/>
+      <c r="AT51" s="8"/>
+      <c r="AU51" s="8"/>
+      <c r="AV51" s="8"/>
+      <c r="AW51" s="8"/>
+      <c r="AX51" s="8"/>
+      <c r="AY51" s="8"/>
+      <c r="AZ51" s="8"/>
+      <c r="BA51" s="8"/>
+      <c r="BB51" s="8"/>
+      <c r="BC51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9" t="n">
         <v>48</v>
       </c>
-      <c r="B52" s="7" t="n">
+      <c r="B52" s="10" t="n">
         <v>0.708333333333333</v>
       </c>
       <c r="C52" s="5"/>
@@ -2962,11 +3335,11 @@
       <c r="BB52" s="6"/>
       <c r="BC52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
+    <row r="53" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="n">
         <v>49</v>
       </c>
-      <c r="B53" s="7" t="n">
+      <c r="B53" s="10" t="n">
         <v>0.715277777777778</v>
       </c>
       <c r="C53" s="5"/>
@@ -3023,11 +3396,11 @@
       <c r="BB53" s="6"/>
       <c r="BC53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
+    <row r="54" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="B54" s="7" t="n">
+      <c r="B54" s="10" t="n">
         <v>0.722222222222222</v>
       </c>
       <c r="C54" s="5"/>
@@ -3084,325 +3457,615 @@
       <c r="BB54" s="6"/>
       <c r="BC54" s="6"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>51</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>0.729166666666667</v>
       </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="W55" s="1"/>
-      <c r="X55" s="1"/>
-      <c r="Y55" s="1"/>
-      <c r="Z55" s="1"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="7"/>
+      <c r="AA55" s="8"/>
+      <c r="AB55" s="8"/>
+      <c r="AC55" s="8"/>
+      <c r="AD55" s="8"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="8"/>
+      <c r="AG55" s="8"/>
+      <c r="AH55" s="8"/>
+      <c r="AI55" s="8"/>
+      <c r="AJ55" s="8"/>
+      <c r="AK55" s="8"/>
+      <c r="AL55" s="8"/>
+      <c r="AM55" s="8"/>
+      <c r="AN55" s="8"/>
+      <c r="AO55" s="8"/>
+      <c r="AP55" s="8"/>
+      <c r="AQ55" s="8"/>
+      <c r="AR55" s="8"/>
+      <c r="AS55" s="8"/>
+      <c r="AT55" s="8"/>
+      <c r="AU55" s="8"/>
+      <c r="AV55" s="8"/>
+      <c r="AW55" s="8"/>
+      <c r="AX55" s="8"/>
+      <c r="AY55" s="8"/>
+      <c r="AZ55" s="8"/>
+      <c r="BA55" s="8"/>
+      <c r="BB55" s="8"/>
+      <c r="BC55" s="8"/>
+    </row>
+    <row r="56" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>52</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>0.736111111111111</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
-      <c r="V56" s="1"/>
-      <c r="W56" s="1"/>
-      <c r="X56" s="1"/>
-      <c r="Y56" s="1"/>
-      <c r="Z56" s="1"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="8"/>
+      <c r="AB56" s="8"/>
+      <c r="AC56" s="8"/>
+      <c r="AD56" s="8"/>
+      <c r="AE56" s="8"/>
+      <c r="AF56" s="8"/>
+      <c r="AG56" s="8"/>
+      <c r="AH56" s="8"/>
+      <c r="AI56" s="8"/>
+      <c r="AJ56" s="8"/>
+      <c r="AK56" s="8"/>
+      <c r="AL56" s="8"/>
+      <c r="AM56" s="8"/>
+      <c r="AN56" s="8"/>
+      <c r="AO56" s="8"/>
+      <c r="AP56" s="8"/>
+      <c r="AQ56" s="8"/>
+      <c r="AR56" s="8"/>
+      <c r="AS56" s="8"/>
+      <c r="AT56" s="8"/>
+      <c r="AU56" s="8"/>
+      <c r="AV56" s="8"/>
+      <c r="AW56" s="8"/>
+      <c r="AX56" s="8"/>
+      <c r="AY56" s="8"/>
+      <c r="AZ56" s="8"/>
+      <c r="BA56" s="8"/>
+      <c r="BB56" s="8"/>
+      <c r="BC56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>0.743055555555556</v>
       </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="1"/>
-      <c r="T57" s="1"/>
-      <c r="U57" s="1"/>
-      <c r="V57" s="1"/>
-      <c r="W57" s="1"/>
-      <c r="X57" s="1"/>
-      <c r="Y57" s="1"/>
-      <c r="Z57" s="1"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
+      <c r="AA57" s="8"/>
+      <c r="AB57" s="8"/>
+      <c r="AC57" s="8"/>
+      <c r="AD57" s="8"/>
+      <c r="AE57" s="8"/>
+      <c r="AF57" s="8"/>
+      <c r="AG57" s="8"/>
+      <c r="AH57" s="8"/>
+      <c r="AI57" s="8"/>
+      <c r="AJ57" s="8"/>
+      <c r="AK57" s="8"/>
+      <c r="AL57" s="8"/>
+      <c r="AM57" s="8"/>
+      <c r="AN57" s="8"/>
+      <c r="AO57" s="8"/>
+      <c r="AP57" s="8"/>
+      <c r="AQ57" s="8"/>
+      <c r="AR57" s="8"/>
+      <c r="AS57" s="8"/>
+      <c r="AT57" s="8"/>
+      <c r="AU57" s="8"/>
+      <c r="AV57" s="8"/>
+      <c r="AW57" s="8"/>
+      <c r="AX57" s="8"/>
+      <c r="AY57" s="8"/>
+      <c r="AZ57" s="8"/>
+      <c r="BA57" s="8"/>
+      <c r="BB57" s="8"/>
+      <c r="BC57" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B58" s="2" t="n">
         <v>0.75</v>
       </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1"/>
-      <c r="W58" s="1"/>
-      <c r="X58" s="1"/>
-      <c r="Y58" s="1"/>
-      <c r="Z58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="7"/>
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="8"/>
+      <c r="AB58" s="8"/>
+      <c r="AC58" s="8"/>
+      <c r="AD58" s="8"/>
+      <c r="AE58" s="8"/>
+      <c r="AF58" s="8"/>
+      <c r="AG58" s="8"/>
+      <c r="AH58" s="8"/>
+      <c r="AI58" s="8"/>
+      <c r="AJ58" s="8"/>
+      <c r="AK58" s="8"/>
+      <c r="AL58" s="8"/>
+      <c r="AM58" s="8"/>
+      <c r="AN58" s="8"/>
+      <c r="AO58" s="8"/>
+      <c r="AP58" s="8"/>
+      <c r="AQ58" s="8"/>
+      <c r="AR58" s="8"/>
+      <c r="AS58" s="8"/>
+      <c r="AT58" s="8"/>
+      <c r="AU58" s="8"/>
+      <c r="AV58" s="8"/>
+      <c r="AW58" s="8"/>
+      <c r="AX58" s="8"/>
+      <c r="AY58" s="8"/>
+      <c r="AZ58" s="8"/>
+      <c r="BA58" s="8"/>
+      <c r="BB58" s="8"/>
+      <c r="BC58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>0.756944444444444</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1"/>
-      <c r="V59" s="1"/>
-      <c r="W59" s="1"/>
-      <c r="X59" s="1"/>
-      <c r="Y59" s="1"/>
-      <c r="Z59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+      <c r="U59" s="7"/>
+      <c r="V59" s="7"/>
+      <c r="W59" s="7"/>
+      <c r="X59" s="7"/>
+      <c r="Y59" s="7"/>
+      <c r="Z59" s="7"/>
+      <c r="AA59" s="8"/>
+      <c r="AB59" s="8"/>
+      <c r="AC59" s="8"/>
+      <c r="AD59" s="8"/>
+      <c r="AE59" s="8"/>
+      <c r="AF59" s="8"/>
+      <c r="AG59" s="8"/>
+      <c r="AH59" s="8"/>
+      <c r="AI59" s="8"/>
+      <c r="AJ59" s="8"/>
+      <c r="AK59" s="8"/>
+      <c r="AL59" s="8"/>
+      <c r="AM59" s="8"/>
+      <c r="AN59" s="8"/>
+      <c r="AO59" s="8"/>
+      <c r="AP59" s="8"/>
+      <c r="AQ59" s="8"/>
+      <c r="AR59" s="8"/>
+      <c r="AS59" s="8"/>
+      <c r="AT59" s="8"/>
+      <c r="AU59" s="8"/>
+      <c r="AV59" s="8"/>
+      <c r="AW59" s="8"/>
+      <c r="AX59" s="8"/>
+      <c r="AY59" s="8"/>
+      <c r="AZ59" s="8"/>
+      <c r="BA59" s="8"/>
+      <c r="BB59" s="8"/>
+      <c r="BC59" s="8"/>
+    </row>
+    <row r="60" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>56</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>0.763888888888889</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="1"/>
-      <c r="W60" s="1"/>
-      <c r="X60" s="1"/>
-      <c r="Y60" s="1"/>
-      <c r="Z60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7"/>
+      <c r="V60" s="7"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="7"/>
+      <c r="Y60" s="7"/>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="8"/>
+      <c r="AB60" s="8"/>
+      <c r="AC60" s="8"/>
+      <c r="AD60" s="8"/>
+      <c r="AE60" s="8"/>
+      <c r="AF60" s="8"/>
+      <c r="AG60" s="8"/>
+      <c r="AH60" s="8"/>
+      <c r="AI60" s="8"/>
+      <c r="AJ60" s="8"/>
+      <c r="AK60" s="8"/>
+      <c r="AL60" s="8"/>
+      <c r="AM60" s="8"/>
+      <c r="AN60" s="8"/>
+      <c r="AO60" s="8"/>
+      <c r="AP60" s="8"/>
+      <c r="AQ60" s="8"/>
+      <c r="AR60" s="8"/>
+      <c r="AS60" s="8"/>
+      <c r="AT60" s="8"/>
+      <c r="AU60" s="8"/>
+      <c r="AV60" s="8"/>
+      <c r="AW60" s="8"/>
+      <c r="AX60" s="8"/>
+      <c r="AY60" s="8"/>
+      <c r="AZ60" s="8"/>
+      <c r="BA60" s="8"/>
+      <c r="BB60" s="8"/>
+      <c r="BC60" s="8"/>
+    </row>
+    <row r="61" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>57</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>0.770833333333333</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-      <c r="T61" s="1"/>
-      <c r="U61" s="1"/>
-      <c r="V61" s="1"/>
-      <c r="W61" s="1"/>
-      <c r="X61" s="1"/>
-      <c r="Y61" s="1"/>
-      <c r="Z61" s="1"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="7"/>
+      <c r="U61" s="7"/>
+      <c r="V61" s="7"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="7"/>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7"/>
+      <c r="AA61" s="8"/>
+      <c r="AB61" s="8"/>
+      <c r="AC61" s="8"/>
+      <c r="AD61" s="8"/>
+      <c r="AE61" s="8"/>
+      <c r="AF61" s="8"/>
+      <c r="AG61" s="8"/>
+      <c r="AH61" s="8"/>
+      <c r="AI61" s="8"/>
+      <c r="AJ61" s="8"/>
+      <c r="AK61" s="8"/>
+      <c r="AL61" s="8"/>
+      <c r="AM61" s="8"/>
+      <c r="AN61" s="8"/>
+      <c r="AO61" s="8"/>
+      <c r="AP61" s="8"/>
+      <c r="AQ61" s="8"/>
+      <c r="AR61" s="8"/>
+      <c r="AS61" s="8"/>
+      <c r="AT61" s="8"/>
+      <c r="AU61" s="8"/>
+      <c r="AV61" s="8"/>
+      <c r="AW61" s="8"/>
+      <c r="AX61" s="8"/>
+      <c r="AY61" s="8"/>
+      <c r="AZ61" s="8"/>
+      <c r="BA61" s="8"/>
+      <c r="BB61" s="8"/>
+      <c r="BC61" s="8"/>
+    </row>
+    <row r="62" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>58</v>
       </c>
       <c r="B62" s="2" t="n">
         <v>0.777777777777778</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1"/>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="1"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="7"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="7"/>
+      <c r="Y62" s="7"/>
+      <c r="Z62" s="7"/>
+      <c r="AA62" s="8"/>
+      <c r="AB62" s="8"/>
+      <c r="AC62" s="8"/>
+      <c r="AD62" s="8"/>
+      <c r="AE62" s="8"/>
+      <c r="AF62" s="8"/>
+      <c r="AG62" s="8"/>
+      <c r="AH62" s="8"/>
+      <c r="AI62" s="8"/>
+      <c r="AJ62" s="8"/>
+      <c r="AK62" s="8"/>
+      <c r="AL62" s="8"/>
+      <c r="AM62" s="8"/>
+      <c r="AN62" s="8"/>
+      <c r="AO62" s="8"/>
+      <c r="AP62" s="8"/>
+      <c r="AQ62" s="8"/>
+      <c r="AR62" s="8"/>
+      <c r="AS62" s="8"/>
+      <c r="AT62" s="8"/>
+      <c r="AU62" s="8"/>
+      <c r="AV62" s="8"/>
+      <c r="AW62" s="8"/>
+      <c r="AX62" s="8"/>
+      <c r="AY62" s="8"/>
+      <c r="AZ62" s="8"/>
+      <c r="BA62" s="8"/>
+      <c r="BB62" s="8"/>
+      <c r="BC62" s="8"/>
+    </row>
+    <row r="63" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B63" s="2" t="n">
         <v>0.784722222222222</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
-      <c r="Z63" s="1"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="7"/>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7"/>
+      <c r="AA63" s="8"/>
+      <c r="AB63" s="8"/>
+      <c r="AC63" s="8"/>
+      <c r="AD63" s="8"/>
+      <c r="AE63" s="8"/>
+      <c r="AF63" s="8"/>
+      <c r="AG63" s="8"/>
+      <c r="AH63" s="8"/>
+      <c r="AI63" s="8"/>
+      <c r="AJ63" s="8"/>
+      <c r="AK63" s="8"/>
+      <c r="AL63" s="8"/>
+      <c r="AM63" s="8"/>
+      <c r="AN63" s="8"/>
+      <c r="AO63" s="8"/>
+      <c r="AP63" s="8"/>
+      <c r="AQ63" s="8"/>
+      <c r="AR63" s="8"/>
+      <c r="AS63" s="8"/>
+      <c r="AT63" s="8"/>
+      <c r="AU63" s="8"/>
+      <c r="AV63" s="8"/>
+      <c r="AW63" s="8"/>
+      <c r="AX63" s="8"/>
+      <c r="AY63" s="8"/>
+      <c r="AZ63" s="8"/>
+      <c r="BA63" s="8"/>
+      <c r="BB63" s="8"/>
+      <c r="BC63" s="8"/>
+    </row>
+    <row r="64" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>60</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1"/>
-      <c r="W64" s="1"/>
-      <c r="X64" s="1"/>
-      <c r="Y64" s="1"/>
-      <c r="Z64" s="1"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+      <c r="Y64" s="7"/>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="8"/>
+      <c r="AB64" s="8"/>
+      <c r="AC64" s="8"/>
+      <c r="AD64" s="8"/>
+      <c r="AE64" s="8"/>
+      <c r="AF64" s="8"/>
+      <c r="AG64" s="8"/>
+      <c r="AH64" s="8"/>
+      <c r="AI64" s="8"/>
+      <c r="AJ64" s="8"/>
+      <c r="AK64" s="8"/>
+      <c r="AL64" s="8"/>
+      <c r="AM64" s="8"/>
+      <c r="AN64" s="8"/>
+      <c r="AO64" s="8"/>
+      <c r="AP64" s="8"/>
+      <c r="AQ64" s="8"/>
+      <c r="AR64" s="8"/>
+      <c r="AS64" s="8"/>
+      <c r="AT64" s="8"/>
+      <c r="AU64" s="8"/>
+      <c r="AV64" s="8"/>
+      <c r="AW64" s="8"/>
+      <c r="AX64" s="8"/>
+      <c r="AY64" s="8"/>
+      <c r="AZ64" s="8"/>
+      <c r="BA64" s="8"/>
+      <c r="BB64" s="8"/>
+      <c r="BC64" s="8"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>